<commit_message>
more NMR fast exchange examples
</commit_message>
<xml_diff>
--- a/input/nmr/dsn.4/carbon_3.xlsx
+++ b/input/nmr/dsn.4/carbon_3.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\расчеты прот\NMR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\data science\chemistry\kev\input\nmr\dsn.4\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770AAFCB-A29D-4892-859C-E8A21D3DE975}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stoich_coefficients" sheetId="2" r:id="rId1"/>
@@ -24,12 +25,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -91,22 +86,22 @@
     <t>Men</t>
   </si>
   <si>
-    <t>С6</t>
-  </si>
-  <si>
-    <t>С3</t>
-  </si>
-  <si>
-    <t>С4</t>
-  </si>
-  <si>
-    <t>С5</t>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -137,10 +132,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -420,7 +414,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -491,7 +485,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -529,11 +523,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G19:G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +558,7 @@
       <c r="A3">
         <v>0.26529543070795769</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>8.8431810235985897E-2</v>
       </c>
       <c r="C3">
@@ -575,7 +569,7 @@
       <c r="A4">
         <v>0.27744285925127404</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>8.7268233785512392E-2</v>
       </c>
       <c r="C4">
@@ -586,7 +580,7 @@
       <c r="A5">
         <v>0.28927477017008868</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>8.6134880099986266E-2</v>
       </c>
       <c r="C5">
@@ -597,7 +591,7 @@
       <c r="A6">
         <v>0.3008032987576516</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>8.503058676537105E-2</v>
       </c>
       <c r="C6">
@@ -608,7 +602,7 @@
       <c r="A7">
         <v>0.31203996586198512</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>8.3954250224037241E-2</v>
       </c>
       <c r="C7">
@@ -619,7 +613,7 @@
       <c r="A8">
         <v>0.32299571628871032</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>8.2904822096236772E-2</v>
       </c>
       <c r="C8">
@@ -630,7 +624,7 @@
       <c r="A9">
         <v>0.33368095435922007</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>8.1881305774061011E-2</v>
       </c>
       <c r="C9">
@@ -641,87 +635,12 @@
       <c r="A10">
         <v>0.34410557686703441</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>8.0882753264621243E-2</v>
       </c>
       <c r="C10">
         <v>0.31065891758425607</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -729,11 +648,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:N1048576"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,7 +1191,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1295,11 +1214,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>